<commit_message>
Added OLS with dichotomous population density
</commit_message>
<xml_diff>
--- a/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
+++ b/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spatial Lag Regression" sheetId="1" r:id="rId1"/>
     <sheet name="Spatial Error Regression" sheetId="2" r:id="rId2"/>
     <sheet name="Spatial Regression Full Models" sheetId="3" r:id="rId3"/>
+    <sheet name="OLS Regression Comparison" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="129">
   <si>
     <t>Queen method (first order) used for contiguity weight matrix.</t>
   </si>
@@ -518,6 +519,49 @@
   </si>
   <si>
     <t>Ordinarly Least Square Full Model</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Full Model 1</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Full Model 2</t>
+  </si>
+  <si>
+    <t>0.4932
+(0.1939)</t>
+  </si>
+  <si>
+    <t>0.8604
+(0.4190)</t>
+  </si>
+  <si>
+    <t>-0.1896
+(0.2010)</t>
+  </si>
+  <si>
+    <t>0.0739
+(0.0489)</t>
+  </si>
+  <si>
+    <t>-5.4e-6
+(7.4e-7)</t>
+  </si>
+  <si>
+    <t>popbinary</t>
+  </si>
+  <si>
+    <t>Population density
+1 - low; 0 - high</t>
+  </si>
+  <si>
+    <t>0.0047
+(0.0225)</t>
+  </si>
+  <si>
+    <t>OLS Regression Models with Poverty as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Table 9</t>
   </si>
 </sst>
 </file>
@@ -593,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -677,6 +721,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,8 +736,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1040,12 +1099,12 @@
       <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1054,34 +1113,34 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32" t="s">
+      <c r="N3" s="30"/>
+      <c r="O3" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="32"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1506,12 +1565,12 @@
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="20"/>
       <c r="F16" s="1"/>
       <c r="G16" s="20"/>
@@ -1526,45 +1585,39 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
@@ -1572,6 +1625,12 @@
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1622,12 +1681,12 @@
       <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1636,34 +1695,34 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32" t="s">
+      <c r="N3" s="30"/>
+      <c r="O3" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="32"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2088,12 +2147,12 @@
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
       <c r="G16" s="20"/>
@@ -2108,44 +2167,39 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -2154,6 +2208,11 @@
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2164,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -2198,12 +2257,12 @@
       <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2212,26 +2271,26 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="32"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2471,7 +2530,9 @@
       <c r="B12" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12">
+        <v>2.1880000000000002</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="17">
         <v>76.759</v>
@@ -2618,12 +2679,12 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="20"/>
       <c r="F18" s="26"/>
       <c r="G18" s="20"/>
@@ -2634,50 +2695,432 @@
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A21:D21"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="F1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="30"/>
+    </row>
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="35">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37">
+        <v>76.759</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37">
+        <v>78.174999999999997</v>
+      </c>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="12">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="12">
+        <v>82.382300000000001</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="12">
+        <v>123.155</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="12">
+        <v>114.09099999999999</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="12">
+        <v>-160.76499999999999</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="12">
+        <v>-234.309</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="12">
+        <v>-216.18299999999999</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="21">
+        <v>91</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="21">
+        <v>91</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="21">
+        <v>91</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Tables for results of modified regression models
</commit_message>
<xml_diff>
--- a/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
+++ b/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="783"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="882" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Spatial Lag Regression" sheetId="1" r:id="rId1"/>
     <sheet name="Spatial Error Regression" sheetId="2" r:id="rId2"/>
     <sheet name="Spatial Regression Full Models" sheetId="3" r:id="rId3"/>
     <sheet name="OLS Regression Comparison" sheetId="4" r:id="rId4"/>
+    <sheet name="Mod OLS Regression Comparison" sheetId="5" r:id="rId5"/>
+    <sheet name="Modified Spatial Regression" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="192">
   <si>
     <t>Queen method (first order) used for contiguity weight matrix.</t>
   </si>
@@ -547,9 +549,6 @@
 (7.4e-7)</t>
   </si>
   <si>
-    <t>popbinary</t>
-  </si>
-  <si>
     <t>Population density
 1 - low; 0 - high</t>
   </si>
@@ -562,6 +561,282 @@
   </si>
   <si>
     <t>Table 9</t>
+  </si>
+  <si>
+    <t>Contiguity Weight Matrix</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Population density
+(ratio variable)</t>
+  </si>
+  <si>
+    <t>0.3481
+(0.0425)</t>
+  </si>
+  <si>
+    <t>0.4430
+(0.3151)</t>
+  </si>
+  <si>
+    <t>-0.0448
+(0.0461)</t>
+  </si>
+  <si>
+    <t>-3.48e-6
+(7.59e-7)</t>
+  </si>
+  <si>
+    <t>6.59e-5
+(1.49e-5)</t>
+  </si>
+  <si>
+    <t>Distance Band</t>
+  </si>
+  <si>
+    <t>0.3209
+(0.0320)</t>
+  </si>
+  <si>
+    <t>0.5120
+(0.3069)</t>
+  </si>
+  <si>
+    <t>-4.00e-6
+(5.28e-7)</t>
+  </si>
+  <si>
+    <t>5.727e-5
+(1.189e-5)</t>
+  </si>
+  <si>
+    <t>F statistic</t>
+  </si>
+  <si>
+    <t>0.3425
+(0.0471)</t>
+  </si>
+  <si>
+    <t>0.5452
+(0.3485)</t>
+  </si>
+  <si>
+    <t>-0.1963
+(0.0356)</t>
+  </si>
+  <si>
+    <t>1.00e-4
+(1.28e-5)</t>
+  </si>
+  <si>
+    <t>0.3823
+(0.0724)</t>
+  </si>
+  <si>
+    <t>1.772
+(0.4231)</t>
+  </si>
+  <si>
+    <t>-0.1962
+(0.0481)</t>
+  </si>
+  <si>
+    <t>-0.0719
+(0.0248)</t>
+  </si>
+  <si>
+    <t>0.3963
+(0.0331)</t>
+  </si>
+  <si>
+    <t>0.9954
+(0.3369)</t>
+  </si>
+  <si>
+    <t>-4.85e-6
+(5.54e-7)</t>
+  </si>
+  <si>
+    <t>-0.0197
+(0.0179)</t>
+  </si>
+  <si>
+    <t>Ordinary Least Square
+Baseline</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 1</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 2</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 3</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 4</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 5</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 6</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 7</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 8</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 9</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 10</t>
+  </si>
+  <si>
+    <t>Table 10</t>
+  </si>
+  <si>
+    <t>Queen method contiguity matrix is first order.</t>
+  </si>
+  <si>
+    <t>Modified OLS Regression Models with Poverty as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Table 11</t>
+  </si>
+  <si>
+    <t>Spatial Regression
+Modified Model 1</t>
+  </si>
+  <si>
+    <t>0.2392
+(0.0718)</t>
+  </si>
+  <si>
+    <t>1.0771
+(0.3788)</t>
+  </si>
+  <si>
+    <t>-0.1261
+(0.0435)</t>
+  </si>
+  <si>
+    <t>-0.0420
+(0.0225)</t>
+  </si>
+  <si>
+    <r>
+      <t>rho (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>lambda (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>λ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>0.5067
+(0.1044)</t>
+  </si>
+  <si>
+    <t>0.4210
+(0.0756)</t>
+  </si>
+  <si>
+    <t>1.019
+(0.3847)</t>
+  </si>
+  <si>
+    <t>-0.1958
+(0.0531)</t>
+  </si>
+  <si>
+    <t>-0.0497
+(0.0292)</t>
+  </si>
+  <si>
+    <t>0.6227
+(0.1069)</t>
+  </si>
+  <si>
+    <t>Distance band contiguity matrix is max-min 14,445 meters.</t>
+  </si>
+  <si>
+    <t>0.2103
+(0.0787)</t>
+  </si>
+  <si>
+    <t>1.0296
+(0.4436)</t>
+  </si>
+  <si>
+    <t>-0.1133
+(0.0427)</t>
+  </si>
+  <si>
+    <t>-0.0369
+(0.0230)</t>
+  </si>
+  <si>
+    <t>0.5729
+(0.1768)</t>
+  </si>
+  <si>
+    <t>-0.1008
+(0.3023)</t>
+  </si>
+  <si>
+    <t>Spatial Error
+Modified Model 1</t>
+  </si>
+  <si>
+    <t>Spatial Lag and Error
+Modified Model 1</t>
   </si>
 </sst>
 </file>
@@ -637,7 +912,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -736,8 +1011,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -747,6 +1022,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1113,34 +1404,34 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34" t="s">
+      <c r="L3" s="38"/>
+      <c r="M3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="38"/>
+      <c r="O3" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="34"/>
+      <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1620,6 +1911,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
@@ -1627,12 +1924,6 @@
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1644,10 +1935,10 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,34 +1988,34 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34" t="s">
+      <c r="L3" s="38"/>
+      <c r="M3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="38"/>
+      <c r="O3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="34"/>
+      <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2204,6 +2495,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -2212,11 +2508,6 @@
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2275,26 +2566,26 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="34"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" spans="1:12" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2734,17 +3025,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2753,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -2764,371 +3055,1795 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="F1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-    </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="34"/>
-    </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="G4" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="17" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="22" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="22" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="17"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="31">
+      <c r="B11" s="31">
         <v>2.1880000000000002</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33">
+      <c r="C11" s="32"/>
+      <c r="D11" s="33">
         <v>76.759</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33">
+      <c r="E11" s="32"/>
+      <c r="F11" s="33">
         <v>78.174999999999997</v>
       </c>
-      <c r="H11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="12">
+        <v>64.751999999999995</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="17">
+        <v>54.953000000000003</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="17">
+        <v>41.957999999999998</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B13" s="12">
         <v>0.42109999999999997</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12">
+      <c r="C13" s="6"/>
+      <c r="D13" s="12">
         <v>0.76400000000000001</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="12">
+      <c r="E13" s="6"/>
+      <c r="F13" s="12">
         <v>0.71199999999999997</v>
       </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B14" s="12">
         <v>82.382300000000001</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12">
+      <c r="C14" s="6"/>
+      <c r="D14" s="12">
         <v>123.155</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="12">
+      <c r="E14" s="6"/>
+      <c r="F14" s="12">
         <v>114.09099999999999</v>
       </c>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B15" s="12">
         <v>-160.76499999999999</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12">
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
         <v>-234.309</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="12">
+      <c r="E15" s="6"/>
+      <c r="F15" s="12">
         <v>-216.18299999999999</v>
       </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="B16" s="12">
         <v>0.19700000000000001</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="12">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="12">
+      <c r="E16" s="6"/>
+      <c r="F16" s="12">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="21">
+      <c r="B17" s="21">
         <v>91</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="21">
+      <c r="C17" s="6"/>
+      <c r="D17" s="21">
         <v>91</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="21">
+      <c r="E17" s="6"/>
+      <c r="F17" s="21">
         <v>91</v>
       </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="29"/>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>2</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>62</v>
       </c>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A17:D17"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="24" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="24" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="24" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="24" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" style="24" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="23" max="23" width="5.7109375" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="W1" s="23"/>
+    </row>
+    <row r="2" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+    </row>
+    <row r="3" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="W3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="22"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="M10" s="32"/>
+      <c r="N10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="S10" s="32"/>
+      <c r="T10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="U10" s="32"/>
+      <c r="V10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="W10" s="32"/>
+    </row>
+    <row r="11" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17">
+        <v>20.920999999999999</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="17">
+        <v>20.920999999999999</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="17">
+        <v>10.698</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="17">
+        <v>10.698</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="17">
+        <v>9.657</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="17">
+        <v>9.657</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="17">
+        <v>15.581</v>
+      </c>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="17">
+        <v>15.581</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="12">
+        <v>64.751999999999995</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="17">
+        <v>69.256</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="17">
+        <v>69.256</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="17">
+        <v>92.087000000000003</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="17">
+        <v>92.087000000000003</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="17">
+        <v>67.942999999999998</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="17">
+        <v>67.942999999999998</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="17">
+        <v>69.427000000000007</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="17">
+        <v>69.427000000000007</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="12">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="12">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="12">
+        <v>0.752</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="12">
+        <v>0.752</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="12">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="12">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="12">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="12">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12">
+        <v>82.382300000000001</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="12">
+        <v>123.033</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="12">
+        <v>123.033</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="12">
+        <v>122.536</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="12">
+        <v>122.536</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="12">
+        <v>112.41800000000001</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="12">
+        <v>112.41800000000001</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="12">
+        <v>113.10899999999999</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="12">
+        <v>113.10899999999999</v>
+      </c>
+      <c r="S14" s="6"/>
+      <c r="T14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-160.76499999999999</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
+        <v>-236.065</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12">
+        <v>-236.065</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="12">
+        <v>-237.07300000000001</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="12">
+        <v>-237.07300000000001</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="12">
+        <v>-216.83600000000001</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="N15" s="12">
+        <v>-216.83600000000001</v>
+      </c>
+      <c r="O15" s="6"/>
+      <c r="P15" s="12">
+        <v>-218.21799999999999</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="12">
+        <v>-218.21799999999999</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="U15" s="6"/>
+      <c r="V15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="12">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="12">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="12">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="12">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="O16" s="6"/>
+      <c r="P16" s="12">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="12">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="S16" s="6"/>
+      <c r="T16" s="12">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="21">
+        <v>91</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="21">
+        <v>91</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="21">
+        <v>91</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="21">
+        <v>91</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="21">
+        <v>91</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="21">
+        <v>91</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="21">
+        <v>91</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="21">
+        <v>91</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="21">
+        <v>91</v>
+      </c>
+      <c r="S17" s="6"/>
+      <c r="T17" s="21">
+        <v>91</v>
+      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="21">
+        <v>91</v>
+      </c>
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="34"/>
+    </row>
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="24" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+    </row>
+    <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="M10" s="32"/>
+    </row>
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="12">
+        <v>64.751999999999995</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="12">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="12">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="12">
+        <v>0.623</v>
+      </c>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12">
+        <v>82.382300000000001</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="12">
+        <v>98.855999999999995</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="12">
+        <v>96.98</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-160.76499999999999</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="12">
+        <v>-187.71199999999999</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="12">
+        <v>-185.96100000000001</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="12">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="12">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="21">
+        <v>91</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="21">
+        <v>91</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="21">
+        <v>91</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="21">
+        <v>91</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="21">
+        <v>91</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="21">
+        <v>91</v>
+      </c>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="34"/>
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Draft of final project paper up to conclusion and critical reflection
</commit_message>
<xml_diff>
--- a/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
+++ b/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="882"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="882" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Spatial Lag Regression" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>Spatial Lag Model 1</t>
   </si>
   <si>
-    <t>Spatial Lag Regression Models with Poverty as Dependent Variable</t>
-  </si>
-  <si>
     <t>Table 6</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
   </si>
   <si>
     <t>Table 7</t>
-  </si>
-  <si>
-    <t>Spatial Error Regression Models with Poverty as Dependent Variable</t>
   </si>
   <si>
     <t>Spatial Error Model 1</t>
@@ -436,9 +430,6 @@
     <t>Table 8</t>
   </si>
   <si>
-    <t>Spatial Regression Models with Poverty as Dependent Variable</t>
-  </si>
-  <si>
     <t>Multicollinearity Condition Number</t>
   </si>
   <si>
@@ -511,9 +502,6 @@
 (0.0225)</t>
   </si>
   <si>
-    <t>OLS Regression Models with Poverty as Dependent Variable</t>
-  </si>
-  <si>
     <t>Table 9</t>
   </si>
   <si>
@@ -661,10 +649,6 @@
   </si>
   <si>
     <t>Table 11</t>
-  </si>
-  <si>
-    <t>Spatial Regression
-Modified Model 1</t>
   </si>
   <si>
     <t>0.2392
@@ -755,9 +739,6 @@
 (0.1069)</t>
   </si>
   <si>
-    <t>Distance band contiguity matrix is max-min 14,445 meters.</t>
-  </si>
-  <si>
     <t>0.2103
 (0.0787)</t>
   </si>
@@ -796,27 +777,7 @@
     <t>Table 13</t>
   </si>
   <si>
-    <t>Spatial Error 
-Full Model 6</t>
-  </si>
-  <si>
-    <t>Spatial Lag 
-Full Model 6</t>
-  </si>
-  <si>
     <t>Spatial Lag and Error Full Model</t>
-  </si>
-  <si>
-    <t>Modified OLS Regression Models with Poverty as Dependent Variable Excluding White Population</t>
-  </si>
-  <si>
-    <t>Modified OLS Regression Models with Poverty as Dependent Variable Excluding White Population and Education Attainment</t>
-  </si>
-  <si>
-    <t>Modified OLS Regression Models with Poverty as Dependent Variable Excluding White Population and Median Household Income</t>
-  </si>
-  <si>
-    <t>Modified Spatial Regression Models with Poverty as Dependent Variable</t>
   </si>
   <si>
     <t>0.3258
@@ -846,6 +807,45 @@
   </si>
   <si>
     <t>Distance band contiguity matrix is max-min 19,445 meters.</t>
+  </si>
+  <si>
+    <t>Spatial Lag 
+Full Model</t>
+  </si>
+  <si>
+    <t>Spatial Error 
+Full Model</t>
+  </si>
+  <si>
+    <t>Spatial Lag
+Modified Model 1</t>
+  </si>
+  <si>
+    <t>Multicollinearity Condition No.</t>
+  </si>
+  <si>
+    <t>Spatial Lag Regression Models with Poverty Ratio as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Spatial Error Regression Models with Poverty Ratio as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Spatial Regression Models with Poverty Ratio as Dependent Variable</t>
+  </si>
+  <si>
+    <t>OLS Regression Models with Poverty Ratio as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Modified OLS Regression Models with Poverty Ratio as Dependent Variable Excluding White Population Ratio</t>
+  </si>
+  <si>
+    <t>Modified OLS Regression Models with Poverty Ratio as Dependent Variable Excluding White Population Ratio and Education Attainment Index</t>
+  </si>
+  <si>
+    <t>Modified OLS Regression Models with Poverty Ratio as Dependent Variable Excluding White Population Ratio and Median Household Income</t>
+  </si>
+  <si>
+    <t>Modified Spatial Regression Models with Poverty Ratio as Dependent Variable</t>
   </si>
 </sst>
 </file>
@@ -921,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1047,9 +1047,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1376,7 +1373,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1393,13 +1395,13 @@
     <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="24" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -1410,90 +1412,90 @@
       <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="47"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="46"/>
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,16 +1503,16 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="6"/>
@@ -1521,7 +1523,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="6"/>
       <c r="N5" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" s="6"/>
     </row>
@@ -1534,10 +1536,10 @@
       <c r="D6" s="12"/>
       <c r="E6" s="6"/>
       <c r="F6" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="6"/>
@@ -1546,7 +1548,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="6"/>
       <c r="N6" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" s="6"/>
     </row>
@@ -1561,7 +1563,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="6"/>
       <c r="H7" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>10</v>
@@ -1571,13 +1573,13 @@
       <c r="L7" s="12"/>
       <c r="M7" s="6"/>
       <c r="N7" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
@@ -1588,18 +1590,18 @@
       <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="6"/>
       <c r="N8" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1617,13 +1619,13 @@
       <c r="J9" s="16"/>
       <c r="K9" s="7"/>
       <c r="L9" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>10</v>
@@ -1636,37 +1638,37 @@
       <c r="B10" s="12"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" s="6"/>
     </row>
@@ -1777,7 +1779,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="12">
         <v>-5.7000000000000002E-2</v>
@@ -1838,11 +1840,11 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="20"/>
       <c r="E16" s="1"/>
       <c r="F16" s="20"/>
@@ -1857,42 +1859,41 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
+      <c r="A18" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:C19"/>
@@ -1931,13 +1932,13 @@
     <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="24" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -1949,86 +1950,86 @@
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
+      <c r="M3" s="46"/>
+      <c r="N3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="47"/>
+      <c r="O3" s="46"/>
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="I4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>10</v>
@@ -2039,16 +2040,16 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="6"/>
@@ -2059,7 +2060,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="6"/>
       <c r="N5" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O5" s="6"/>
     </row>
@@ -2072,10 +2073,10 @@
       <c r="D6" s="12"/>
       <c r="E6" s="6"/>
       <c r="F6" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="6"/>
@@ -2084,7 +2085,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="6"/>
       <c r="N6" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O6" s="6"/>
     </row>
@@ -2099,23 +2100,23 @@
       <c r="F7" s="12"/>
       <c r="G7" s="6"/>
       <c r="H7" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="6"/>
       <c r="L7" s="12"/>
       <c r="M7" s="6"/>
       <c r="N7" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
@@ -2126,18 +2127,18 @@
       <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="6"/>
       <c r="N8" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2155,56 +2156,56 @@
       <c r="J9" s="16"/>
       <c r="K9" s="7"/>
       <c r="L9" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O10" s="6"/>
     </row>
@@ -2315,7 +2316,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="12">
         <v>-2.1999999999999999E-2</v>
@@ -2395,15 +2396,15 @@
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -2443,7 +2444,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -2466,7 +2467,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -2476,66 +2477,66 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="K3" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K4" s="18"/>
     </row>
@@ -2544,25 +2545,25 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -2573,19 +2574,19 @@
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -2596,51 +2597,51 @@
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
       <c r="D8" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,25 +2651,25 @@
       <c r="B9" s="15"/>
       <c r="C9" s="7"/>
       <c r="D9" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>10</v>
@@ -2683,13 +2684,13 @@
       <c r="D10" s="17"/>
       <c r="E10" s="6"/>
       <c r="F10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="17"/>
       <c r="I10" s="6"/>
       <c r="J10" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>10</v>
@@ -2697,7 +2698,7 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="6"/>
@@ -2705,17 +2706,17 @@
       <c r="E11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="B12" s="31">
         <v>2.1880000000000002</v>
@@ -2803,7 +2804,7 @@
       <c r="J15" s="12"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>5</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="12">
         <v>8.0000000000000002E-3</v>
@@ -2869,15 +2870,15 @@
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -2934,57 +2935,57 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
       <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,20 +2993,20 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3015,11 +3016,11 @@
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -3030,41 +3031,41 @@
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
       <c r="D8" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>10</v>
@@ -3074,20 +3075,20 @@
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
       <c r="E10" s="6"/>
       <c r="F10" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="31">
         <v>2.1880000000000002</v>
@@ -3104,25 +3105,25 @@
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="12">
         <v>64.751999999999995</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="17">
         <v>54.953000000000003</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="17">
         <v>41.957999999999998</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3185,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="12">
         <v>8.0000000000000002E-3</v>
@@ -3224,15 +3225,15 @@
       <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -3252,8 +3253,7 @@
       <c r="C22" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:C2"/>
+  <mergeCells count="4">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A19:C19"/>
@@ -3292,7 +3292,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -3300,69 +3300,69 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="K3" s="47"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3370,27 +3370,27 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="17" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>10</v>
@@ -3403,70 +3403,70 @@
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="22" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="22" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="6"/>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="6"/>
@@ -3484,42 +3484,42 @@
       <c r="F9" s="17"/>
       <c r="G9" s="6"/>
       <c r="H9" s="22" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="22" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I10" s="32"/>
       <c r="J10" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="12">
         <v>2.1880000000000002</v>
@@ -3544,37 +3544,37 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="12">
         <v>64.751999999999995</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="17">
         <v>69.256</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="17">
         <v>69.256</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="17">
         <v>52.356000000000002</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="17">
         <v>52.356000000000002</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="12">
         <v>-7.0000000000000001E-3</v>
@@ -3720,15 +3720,15 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -3742,14 +3742,14 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3794,7 +3794,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -3804,69 +3804,69 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3874,27 +3874,27 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>10</v>
@@ -3902,52 +3902,52 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="6"/>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
@@ -3965,42 +3965,42 @@
       <c r="F8" s="17"/>
       <c r="G8" s="6"/>
       <c r="H8" s="22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I9" s="32"/>
       <c r="J9" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B10" s="12">
         <v>2.1880000000000002</v>
@@ -4025,37 +4025,37 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B11" s="12">
         <v>64.751999999999995</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="17">
         <v>92.087000000000003</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="17">
         <v>92.087000000000003</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="17">
         <v>67.942999999999998</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="17">
         <v>67.942999999999998</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -4201,15 +4201,15 @@
       <c r="K17" s="35"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -4223,14 +4223,14 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4275,7 +4275,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -4285,69 +4285,69 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="K3" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="I4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="K4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4355,30 +4355,30 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4388,47 +4388,47 @@
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="I6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>133</v>
-      </c>
       <c r="K6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="6"/>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
@@ -4446,13 +4446,13 @@
       <c r="F8" s="17"/>
       <c r="G8" s="6"/>
       <c r="H8" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>10</v>
@@ -4460,32 +4460,32 @@
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I9" s="32"/>
       <c r="J9" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B10" s="12">
         <v>2.1880000000000002</v>
@@ -4510,37 +4510,37 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B11" s="12">
         <v>64.751999999999995</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="17">
         <v>69.427000000000007</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="17">
         <v>69.427000000000007</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="17">
         <v>29.805</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="17">
         <v>29.805</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="12">
         <v>1.0999999999999999E-2</v>
@@ -4640,7 +4640,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="12">
         <v>-0.01</v>
@@ -4688,15 +4688,15 @@
       <c r="K17" s="35"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -4710,14 +4710,14 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4738,7 +4738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -4764,7 +4764,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -4775,76 +4775,76 @@
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47" t="s">
-        <v>173</v>
-      </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="M3" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>167</v>
       </c>
       <c r="M4" s="18" t="s">
         <v>10</v>
@@ -4855,40 +4855,40 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4898,31 +4898,31 @@
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>10</v>
@@ -4930,38 +4930,38 @@
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="32"/>
@@ -4970,15 +4970,15 @@
       <c r="F8" s="41"/>
       <c r="G8" s="32"/>
       <c r="H8" s="41" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I8" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="41"/>
       <c r="K8" s="32"/>
       <c r="L8" s="41" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>10</v>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="6"/>
@@ -4997,48 +4997,48 @@
       <c r="H9" s="22"/>
       <c r="I9" s="40"/>
       <c r="J9" s="22" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I10" s="32"/>
       <c r="J10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K10" s="32"/>
       <c r="L10" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M10" s="32"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="12">
         <v>2.1880000000000002</v>
@@ -5061,25 +5061,25 @@
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="12">
         <v>64.751999999999995</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="17">
         <v>29.805</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="17">
         <v>29.805</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="6"/>
@@ -5179,13 +5179,13 @@
         <v>0.19700000000000001</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="12">
         <v>0.22600000000000001</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="12">
         <v>-0.01</v>
@@ -5249,15 +5249,15 @@
       <c r="M18" s="34"/>
     </row>
     <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -5271,14 +5271,14 @@
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added analyis of White population and conclusion to paper for Final Project
</commit_message>
<xml_diff>
--- a/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
+++ b/Assignments/Homework02/docs/Townes_SOC5670_Homework02_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="882" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="882" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Spatial Lag Regression" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Mod OLS Regression - MHI" sheetId="7" r:id="rId6"/>
     <sheet name="Mod OLS Regression - Educ" sheetId="8" r:id="rId7"/>
     <sheet name="Modified Spatial Regression" sheetId="6" r:id="rId8"/>
+    <sheet name="Modified Spatial Regression 2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="236">
   <si>
     <t>Queen method (first order) used for contiguity weight matrix.</t>
   </si>
@@ -846,6 +847,178 @@
   </si>
   <si>
     <t>Modified Spatial Regression Models with Poverty Ratio as Dependent Variable</t>
+  </si>
+  <si>
+    <t>Ordinary Least Square
+Baseline 2</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 13</t>
+  </si>
+  <si>
+    <t>Ordinarly Least Square Modified Model 14</t>
+  </si>
+  <si>
+    <t>Spatial Lag
+Modified Model 2</t>
+  </si>
+  <si>
+    <t>Spatial Error
+Modified Model 2</t>
+  </si>
+  <si>
+    <t>Spatial Lag and Error
+Modified Model 2</t>
+  </si>
+  <si>
+    <t>Table 14</t>
+  </si>
+  <si>
+    <t>Modified Spatial Regression Models with Poverty Ratio as Dependent Variable and White Polulation Ratio as Primary Explanatory Variable of Interest</t>
+  </si>
+  <si>
+    <t>0.3440
+(0.0335)</t>
+  </si>
+  <si>
+    <t>-3.50e-5
+(6.89e-6)</t>
+  </si>
+  <si>
+    <t>0.5864
+(0.0609)</t>
+  </si>
+  <si>
+    <t>-1.49e-5
+(7.01e-6)</t>
+  </si>
+  <si>
+    <t>-0.2286
+(0.4830)</t>
+  </si>
+  <si>
+    <t>-0.1086
+(0.0244)</t>
+  </si>
+  <si>
+    <t>0.3279
+(0.0667)</t>
+  </si>
+  <si>
+    <t>-4.46e-6
+(5.88e-6)</t>
+  </si>
+  <si>
+    <t>-0.1611
+(0.0426)</t>
+  </si>
+  <si>
+    <t>-0.0646
+(0.0218)</t>
+  </si>
+  <si>
+    <t>0.5782
+(0.0998)</t>
+  </si>
+  <si>
+    <t>0.4928
+(0.0755)</t>
+  </si>
+  <si>
+    <t>1.30e-6
+(6.16e-6)</t>
+  </si>
+  <si>
+    <t>-0.2352
+(0.0571)</t>
+  </si>
+  <si>
+    <t>-0.0554
+(0.0305)</t>
+  </si>
+  <si>
+    <t>0.7265
+(0.0877)</t>
+  </si>
+  <si>
+    <t>0.9572
+(0.1707)</t>
+  </si>
+  <si>
+    <t>0.3323
+(0.1965)</t>
+  </si>
+  <si>
+    <t>-0.1500
+(0.0480)</t>
+  </si>
+  <si>
+    <t>-0.0314
+(0.0278)</t>
+  </si>
+  <si>
+    <t>-0.7080
+(0.1760)</t>
+  </si>
+  <si>
+    <t>0.3804
+(0.2564)</t>
+  </si>
+  <si>
+    <t>0.9568
+(0.2200)</t>
+  </si>
+  <si>
+    <t>-0.7092
+(0.2222)</t>
+  </si>
+  <si>
+    <t>-0.1491
+(0.0463)</t>
+  </si>
+  <si>
+    <t>-0.0316
+(0.0162)</t>
+  </si>
+  <si>
+    <t>0.3344
+(0.1839)</t>
+  </si>
+  <si>
+    <t>0.3395
+(0.2936)</t>
+  </si>
+  <si>
+    <t>Spatial Lag and Error
+Modified Model 2(HET)</t>
+  </si>
+  <si>
+    <t>Spatial Lag and Error
+Modified Model 1(HET)</t>
+  </si>
+  <si>
+    <t>0.2093
+(0.0733)</t>
+  </si>
+  <si>
+    <t>1.0326
+(0.5007)</t>
+  </si>
+  <si>
+    <t>-0.1127
+(0.0428)</t>
+  </si>
+  <si>
+    <t>-0.0368
+(0.0151)</t>
+  </si>
+  <si>
+    <t>0.5733
+(0.1544)</t>
+  </si>
+  <si>
+    <t>-0.0539
+(0.3195)</t>
   </si>
 </sst>
 </file>
@@ -921,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1051,11 +1224,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1422,34 +1601,34 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="46"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1840,11 +2019,11 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="20"/>
       <c r="E16" s="1"/>
       <c r="F16" s="20"/>
@@ -1859,47 +2038,47 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1959,34 +2138,34 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="46"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2396,11 +2575,11 @@
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
@@ -2486,26 +2665,26 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="K3" s="46"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2870,11 +3049,11 @@
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
@@ -2952,18 +3131,18 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3225,11 +3404,11 @@
       <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
@@ -3309,26 +3488,26 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="46"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3720,11 +3899,11 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
@@ -3813,26 +3992,26 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="46"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -4201,11 +4380,11 @@
       <c r="K17" s="35"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
@@ -4294,26 +4473,26 @@
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="46"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -4688,11 +4867,11 @@
       <c r="K17" s="35"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
@@ -4736,7 +4915,633 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="24" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="O1" s="23"/>
+    </row>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+    </row>
+    <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" s="45"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" s="12"/>
+      <c r="N7" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="41"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" s="32"/>
+      <c r="N10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="32"/>
+    </row>
+    <row r="11" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="17">
+        <v>16.690999999999999</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="12">
+        <v>64.751999999999995</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="17">
+        <v>29.805</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="12">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="12">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="12">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="12">
+        <v>0.623</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="12">
+        <v>0.623</v>
+      </c>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12">
+        <v>82.382300000000001</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="12">
+        <v>89.673000000000002</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="12">
+        <v>98.855999999999995</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="12">
+        <v>96.98</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-160.76499999999999</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12">
+        <v>-171.345</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="12">
+        <v>-187.71199999999999</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="12">
+        <v>-185.96100000000001</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="12">
+        <v>-0.01</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="12">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="12">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="21">
+        <v>91</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="21">
+        <v>91</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="21">
+        <v>91</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="21">
+        <v>91</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="21">
+        <v>91</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="21">
+        <v>91</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="21">
+        <v>91</v>
+      </c>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="44"/>
+    </row>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -4760,11 +5565,13 @@
     <col min="11" max="11" width="5.7109375" style="24" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="C1" s="19"/>
       <c r="E1" s="23"/>
@@ -4772,194 +5579,219 @@
       <c r="I1" s="23"/>
       <c r="K1" s="23"/>
       <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="23"/>
+    </row>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
     </row>
-    <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46" t="s">
-        <v>168</v>
-      </c>
-      <c r="M3" s="46"/>
-    </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="O3" s="45"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>149</v>
+        <v>206</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>23</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="M4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="22" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N6" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="22" t="s">
-        <v>130</v>
+        <v>205</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="I7" s="12"/>
       <c r="J7" s="22" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="22" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>153</v>
       </c>
@@ -4970,21 +5802,23 @@
       <c r="F8" s="41"/>
       <c r="G8" s="32"/>
       <c r="H8" s="41" t="s">
-        <v>155</v>
+        <v>210</v>
       </c>
       <c r="I8" s="42" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="41"/>
       <c r="K8" s="32"/>
-      <c r="L8" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="M8" s="32"/>
+      <c r="N8" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="O8" s="32"/>
+    </row>
+    <row r="9" spans="1:15" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>154</v>
       </c>
@@ -4997,17 +5831,21 @@
       <c r="H9" s="22"/>
       <c r="I9" s="40"/>
       <c r="J9" s="22" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
       <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>108</v>
       </c>
@@ -5035,21 +5873,25 @@
         <v>109</v>
       </c>
       <c r="M10" s="32"/>
-    </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="32"/>
+    </row>
+    <row r="11" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="12">
-        <v>2.1880000000000002</v>
+        <v>5.4020000000000001</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="17">
-        <v>16.690999999999999</v>
+        <v>15.119</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="17">
-        <v>16.690999999999999</v>
+        <v>15.119</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="17"/>
@@ -5058,25 +5900,27 @@
       <c r="K11" s="6"/>
       <c r="L11" s="17"/>
       <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="17"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>122</v>
       </c>
       <c r="B12" s="12">
-        <v>64.751999999999995</v>
+        <v>25.826000000000001</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="17">
-        <v>29.805</v>
+        <v>22.471</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="17">
-        <v>29.805</v>
+        <v>22.471</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>23</v>
@@ -5087,122 +5931,134 @@
       <c r="K12" s="6"/>
       <c r="L12" s="17"/>
       <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="17"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="12">
-        <v>0.42109999999999997</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="12">
-        <v>0.50700000000000001</v>
+        <v>0.437</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="12">
-        <v>0.50700000000000001</v>
+        <v>0.437</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="12">
-        <v>0.61799999999999999</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="12">
-        <v>0.61399999999999999</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="12">
-        <v>0.623</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="12">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="12">
-        <v>82.382300000000001</v>
+        <v>69.010000000000005</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="12">
-        <v>89.673000000000002</v>
+        <v>83.611000000000004</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="12">
-        <v>89.673000000000002</v>
+        <v>83.611000000000004</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="12">
-        <v>98.855999999999995</v>
+        <v>95.393000000000001</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="12">
-        <v>96.98</v>
+        <v>93.983999999999995</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="12"/>
       <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="12"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="12">
-        <v>-160.76499999999999</v>
+        <v>-134.19999999999999</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="12">
-        <v>-171.345</v>
+        <v>-159.22300000000001</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="12">
-        <v>-171.345</v>
+        <v>-159.22300000000001</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="12">
-        <v>-187.71199999999999</v>
+        <v>-180.786</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="12">
-        <v>-185.96100000000001</v>
+        <v>-179.96799999999999</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="12"/>
       <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="12"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="12">
-        <v>0.19700000000000001</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="12">
-        <v>0.22600000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="12">
-        <v>-0.01</v>
+      <c r="F16" s="27">
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="12">
-        <v>-5.0000000000000001E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="12">
-        <v>-1.0999999999999999E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="12"/>
       <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="12"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>4</v>
       </c>
@@ -5230,66 +6086,73 @@
         <v>91</v>
       </c>
       <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="21">
+        <v>91</v>
+      </c>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="34"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="34"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="34"/>
+      <c r="K18" s="44"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="34"/>
-    </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="M18" s="44"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="44"/>
+    </row>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>147</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="L3:M3"/>
+  <mergeCells count="8">
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A19:C19"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>